<commit_message>
gifs and mp4s uploaded
</commit_message>
<xml_diff>
--- a/Sales Funnel Analysis in Power BI/SalesFunnelData.xlsx
+++ b/Sales Funnel Analysis in Power BI/SalesFunnelData.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Medium Articles\DRAFT\Sales Funnel Analysis in Power BI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0E60CF-BC03-4D35-926E-48842563A185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B912D34C-FFC6-4D6C-8C8E-F4886693B9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3DA5C9B6-D555-4F4F-B57C-DA690E75EF90}"/>
   </bookViews>
   <sheets>
-    <sheet name="funneldata" sheetId="1" r:id="rId1"/>
+    <sheet name="SalesFunnelData" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">funneldata!$A$1:$G$176</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SalesFunnelData!$A$1:$G$176</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1733,7 +1733,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D206" sqref="D206"/>
+      <selection pane="bottomLeft" activeCell="N205" sqref="N205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>